<commit_message>
Update NRSC_StudentInfo.xlsx with new data for student information processing
</commit_message>
<xml_diff>
--- a/servers/emails/out/templates/assets/NRSC_StudentInfo.xlsx
+++ b/servers/emails/out/templates/assets/NRSC_StudentInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DevDrive/NRSC/StudentApplicationPipeline/servers/emails/out/templates/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60743DBE-3561-9740-97A1-EF638F2FA940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551B898-7F78-F840-8DD2-EF316BEBD41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{E031096F-700E-654A-AB6C-FCF4303436DA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>PERSONAL INFORMATION</t>
   </si>
@@ -61,9 +61,6 @@
     <t>[Enter date of birth]</t>
   </si>
   <si>
-    <t>2000-01-15 (YYYY-MM-DD)</t>
-  </si>
-  <si>
     <t>ACADEMIC INFORMATION</t>
   </si>
   <si>
@@ -346,12 +343,6 @@
   </si>
   <si>
     <t xml:space="preserve"> (minimum 60%)</t>
-  </si>
-  <si>
-    <t>2025-12-15 (required )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-15 (at least 15 days from today) </t>
   </si>
   <si>
     <r>
@@ -414,13 +405,31 @@
       </rPr>
       <t xml:space="preserve"> for internship</t>
     </r>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-08-2024 (at least 15 days from today) </t>
+  </si>
+  <si>
+    <t>15-12-2024 (required )</t>
+  </si>
+  <si>
+    <t>15-08-2000 (DD-MM-YYYY)</t>
+  </si>
+  <si>
+    <t>2. For Degree Type, please copy paste the full option into the box to allow our systems to validate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Duration Preference should be filled in numeric values only, no days or months suffix. Eg. (45,3,4) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,6 +561,26 @@
       <u/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -576,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -602,11 +631,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -644,11 +754,49 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,14 +1172,15 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1072,16 +1221,25 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-    </row>
-    <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -1090,14 +1248,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>3</v>
@@ -1106,11 +1269,19 @@
         <v>4</v>
       </c>
       <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>5</v>
@@ -1119,229 +1290,270 @@
         <v>6</v>
       </c>
       <c r="D7" s="16"/>
-      <c r="E7" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>9</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="B11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="19" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="19" t="s">
-        <v>17</v>
-      </c>
       <c r="D15" s="16"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="11"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="C17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="C18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
         <v>24</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>25</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>49</v>
@@ -1352,28 +1564,28 @@
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="18"/>
@@ -1381,25 +1593,25 @@
       <c r="G25" s="10"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="10"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
       <c r="G27" s="10"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
@@ -1407,14 +1619,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="B11:B15"/>
+    <mergeCell ref="E5:J5"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>